<commit_message>
Trying to post on github pages
</commit_message>
<xml_diff>
--- a/Project Logs/Project_Log.xlsx
+++ b/Project Logs/Project_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acedskillz/ActivityFinder/Project Logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B96BAB-3490-3548-BABE-4D4027F04461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18828E72-A38A-FF49-B92A-0315A1E715C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="760" windowWidth="22200" windowHeight="16780" xr2:uid="{85DCD83A-61FC-594B-B261-D866B9130835}"/>
+    <workbookView xWindow="9180" yWindow="500" windowWidth="24700" windowHeight="16780" xr2:uid="{85DCD83A-61FC-594B-B261-D866B9130835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="218">
   <si>
     <t>Date</t>
   </si>
@@ -666,6 +666,30 @@
   </si>
   <si>
     <t>Removed old files and pushed the new log</t>
+  </si>
+  <si>
+    <t>6hr   Preparing documentation for presentation</t>
+  </si>
+  <si>
+    <t>Goals: Get planned APIs onto page, functioning in its proper way Challenges: Getting that geocoding to get current location causes issues that keep retreiving the location</t>
+  </si>
+  <si>
+    <t>Goals: To get the infromation from the google map results and be able to interact with them. Challenges: Getting the data outside of the init method was not useable without return, I had to figure out how I'd place the data into an object</t>
+  </si>
+  <si>
+    <t>Goals: Simulate a search that retreives multiple locations and markers onto the map and lists Challenges: Ran into the road block of money. Had to determine whether I would be spending money to run this project or not.</t>
+  </si>
+  <si>
+    <t>Goals: Configure Yelp API onto page and display results in a pleasing way.  Challenges: Had to figure out how to use grid layout and perform css i never got into learning before</t>
+  </si>
+  <si>
+    <t>Goals: Expand upon express server idea and continue in using mock data for the page. Challenges: Refershing my knowledge on Express was a bit of a challenge that still needs to be worked upon</t>
+  </si>
+  <si>
+    <t>Goals: Needed to fall upon final design of Yelp results and make sure of consistency with data Challenges: Creating a blurred background for the image of the restaurant was a cool idea but dove into css i had to learn such as element positioning and z index</t>
+  </si>
+  <si>
+    <t>Goals: Get a fairly simple/minimal express server running Challenges: Understanding how to make a request along with my passed header apikey didn't make much sense at all. There was some coode I didn't understand and desire to find something more simple.</t>
   </si>
 </sst>
 </file>
@@ -762,7 +786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -786,19 +810,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -809,16 +820,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1138,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB482F63-C323-E046-AB4D-CC5688187403}">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,34 +1173,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1239,32 +1259,32 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -1365,14 +1385,14 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
@@ -1383,14 +1403,14 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
@@ -1520,14 +1540,14 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
@@ -1537,7 +1557,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" s="12" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="13" t="s">
         <v>71</v>
       </c>
@@ -1667,24 +1687,24 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
+      <c r="A38" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:6" s="12" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="13" t="s">
         <v>93</v>
       </c>
@@ -1817,24 +1837,24 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
+      <c r="A48" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-    </row>
-    <row r="50" spans="1:6" s="12" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+    </row>
+    <row r="50" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="13" t="s">
         <v>95</v>
       </c>
@@ -1955,14 +1975,14 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
+      <c r="A58" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
@@ -1972,7 +1992,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" s="12" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="13" t="s">
         <v>96</v>
       </c>
@@ -2075,14 +2095,14 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
+      <c r="A68" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
@@ -2092,15 +2112,15 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="1:6" s="17" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="19" t="s">
+    <row r="70" spans="1:6" s="12" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
     </row>
     <row r="71" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
@@ -2186,32 +2206,32 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
+      <c r="A78" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
     </row>
     <row r="80" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
     </row>
     <row r="81" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
@@ -2250,7 +2270,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>45008</v>
       </c>
@@ -2272,7 +2292,7 @@
         <v>45009</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>45010</v>
       </c>
@@ -2300,32 +2320,32 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10"/>
+      <c r="A88" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
     </row>
     <row r="89" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="11"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
     </row>
     <row r="90" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="9"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
     </row>
     <row r="91" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
@@ -2423,32 +2443,32 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
+      <c r="A98" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
     </row>
     <row r="99" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="11"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="A99" s="16"/>
+      <c r="B99" s="16"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
     </row>
     <row r="100" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="9"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
@@ -2533,7 +2553,7 @@
       <c r="A109" s="4">
         <v>45028</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="15" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2541,31 +2561,31 @@
       <c r="A110" s="4">
         <v>45029</v>
       </c>
-      <c r="B110" s="21"/>
+      <c r="B110" s="15"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>45030</v>
       </c>
-      <c r="B111" s="21"/>
+      <c r="B111" s="15"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>45031</v>
       </c>
-      <c r="B112" s="21"/>
+      <c r="B112" s="15"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>45032</v>
       </c>
-      <c r="B113" s="21"/>
+      <c r="B113" s="15"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>45033</v>
       </c>
-      <c r="B114" s="21"/>
+      <c r="B114" s="15"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
@@ -2591,14 +2611,14 @@
       <c r="F118" s="8"/>
     </row>
     <row r="119" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="9" t="s">
+      <c r="A119" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B119" s="9"/>
-      <c r="C119" s="9"/>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="9"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
     </row>
     <row r="120" spans="1:6" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
@@ -2726,32 +2746,32 @@
       </c>
     </row>
     <row r="127" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
-      <c r="F127" s="10"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="14"/>
     </row>
     <row r="128" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="11"/>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
+      <c r="A128" s="16"/>
+      <c r="B128" s="16"/>
+      <c r="C128" s="16"/>
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="16"/>
     </row>
     <row r="129" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A129" s="20" t="s">
+      <c r="A129" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="10"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+      <c r="F129" s="14"/>
     </row>
     <row r="130" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
@@ -2870,14 +2890,14 @@
       </c>
     </row>
     <row r="137" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="10" t="s">
+      <c r="A137" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B137" s="10"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="10"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="14"/>
+      <c r="D137" s="14"/>
+      <c r="E137" s="14"/>
+      <c r="F137" s="14"/>
     </row>
     <row r="138" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="6"/>
@@ -2888,14 +2908,14 @@
       <c r="F138" s="8"/>
     </row>
     <row r="139" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A139" s="20" t="s">
+      <c r="A139" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B139" s="10"/>
-      <c r="C139" s="10"/>
-      <c r="D139" s="10"/>
-      <c r="E139" s="10"/>
-      <c r="F139" s="10"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
     </row>
     <row r="140" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
@@ -2915,7 +2935,7 @@
       <c r="A141" s="4">
         <v>45052</v>
       </c>
-      <c r="B141" s="21" t="s">
+      <c r="B141" s="15" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2923,13 +2943,13 @@
       <c r="A142" s="4">
         <v>45053</v>
       </c>
-      <c r="B142" s="21"/>
+      <c r="B142" s="15"/>
     </row>
     <row r="143" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>45054</v>
       </c>
-      <c r="B143" s="21"/>
+      <c r="B143" s="15"/>
       <c r="D143" s="2" t="s">
         <v>209</v>
       </c>
@@ -2938,44 +2958,49 @@
       <c r="A144" s="4">
         <v>45055</v>
       </c>
+      <c r="B144" s="15" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="145" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>45056</v>
       </c>
+      <c r="B145" s="15"/>
     </row>
     <row r="146" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>45057</v>
       </c>
+      <c r="B146" s="15"/>
     </row>
     <row r="147" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="10" t="s">
+      <c r="A147" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B147" s="10"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10"/>
-      <c r="E147" s="10"/>
-      <c r="F147" s="10"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="14"/>
     </row>
     <row r="148" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="11"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
+      <c r="A148" s="16"/>
+      <c r="B148" s="16"/>
+      <c r="C148" s="16"/>
+      <c r="D148" s="16"/>
+      <c r="E148" s="16"/>
+      <c r="F148" s="16"/>
     </row>
     <row r="149" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="9" t="s">
+      <c r="A149" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B149" s="9"/>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="9"/>
-      <c r="F149" s="9"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
     </row>
     <row r="150" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
@@ -3003,7 +3028,36 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="39">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A79:F79"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A99:F99"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A119:F119"/>
+    <mergeCell ref="A127:F127"/>
     <mergeCell ref="A149:F149"/>
     <mergeCell ref="A137:F137"/>
     <mergeCell ref="B109:B114"/>
@@ -3013,35 +3067,7 @@
     <mergeCell ref="A139:F139"/>
     <mergeCell ref="A147:F147"/>
     <mergeCell ref="A148:F148"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A99:F99"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A119:F119"/>
-    <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A79:F79"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B144:B146"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>